<commit_message>
update fund net value, and so on.
</commit_message>
<xml_diff>
--- a/ExplorerFund/NetValue/fund record.xlsx
+++ b/ExplorerFund/NetValue/fund record.xlsx
@@ -99,15 +99,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
-    <numFmt numFmtId="176" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.0000_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0.0_ "/>
-    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="180" formatCode="0.0000_ "/>
+    <numFmt numFmtId="179" formatCode="#,##0.0_ "/>
+    <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -134,14 +134,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,7 +195,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -171,6 +203,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -178,7 +218,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,16 +239,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,54 +271,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,49 +286,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,133 +460,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,78 +477,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -569,6 +497,69 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -577,6 +568,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -585,10 +585,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -597,133 +597,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -731,46 +731,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="57" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="57" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1117,8 +1117,8 @@
   <sheetPr/>
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1700,6 +1700,45 @@
         <v>1.1842</v>
       </c>
     </row>
+    <row r="15" spans="1:18">
+      <c r="A15">
+        <v>20161230</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2854917.61</v>
+      </c>
+      <c r="C15" s="3">
+        <v>356418.02</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1329706.14</v>
+      </c>
+      <c r="F15" s="3">
+        <v>712025.26</v>
+      </c>
+      <c r="G15" s="3">
+        <v>456768.19</v>
+      </c>
+      <c r="H15"/>
+      <c r="M15" s="12">
+        <v>1212629.43</v>
+      </c>
+      <c r="N15" s="3">
+        <v>800000</v>
+      </c>
+      <c r="O15" s="1">
+        <v>1.5158</v>
+      </c>
+      <c r="P15" s="3">
+        <v>1642288.17</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>1358019.5</v>
+      </c>
+      <c r="R15" s="1">
+        <v>1.2093</v>
+      </c>
+    </row>
     <row r="17" spans="2:9">
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
@@ -1792,11 +1831,14 @@
       <c r="E30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:16">
       <c r="B31" s="8"/>
       <c r="C31" s="3"/>
       <c r="E31" s="3"/>
       <c r="I31" s="3"/>
+      <c r="P31">
+        <v>30.3</v>
+      </c>
     </row>
     <row r="32" spans="2:9">
       <c r="B32" s="8"/>

</xml_diff>

<commit_message>
backup production environment of JinRui
</commit_message>
<xml_diff>
--- a/ExplorerFund/NetValue/fund record.xlsx
+++ b/ExplorerFund/NetValue/fund record.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
   <si>
     <t>日期</t>
   </si>
@@ -28,7 +28,7 @@
     <t>大连夜盘权益</t>
   </si>
   <si>
-    <t>上期日盘权益</t>
+    <t>上期日盘权益19</t>
   </si>
   <si>
     <t>上期夜盘权益63</t>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>小计</t>
+  </si>
+  <si>
+    <t>2017年前结算</t>
   </si>
 </sst>
 </file>
@@ -108,13 +111,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
+    <numFmt numFmtId="176" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.0000_);[Red]\(0.0000\)"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="#,##0.0_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="178" formatCode="#,##0.0_ "/>
     <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="180" formatCode="0.0000_ "/>
   </numFmts>
@@ -143,25 +146,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -172,16 +159,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -196,55 +190,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,6 +219,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
@@ -271,8 +258,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,6 +273,21 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -295,187 +298,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,17 +492,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -514,31 +517,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -564,16 +552,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -594,149 +597,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -749,24 +752,33 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -777,6 +789,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1101,7 +1116,7 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:T21"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1159,7 +1174,7 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="L1" t="s">
@@ -1314,7 +1329,7 @@
       <c r="R4" s="3">
         <v>822018.44</v>
       </c>
-      <c r="S4" s="15">
+      <c r="S4" s="19">
         <f>0.0868942855166899+1</f>
         <v>1.08689428551669</v>
       </c>
@@ -1336,11 +1351,11 @@
       <c r="M5" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="11"/>
+      <c r="N5" s="14"/>
       <c r="O5" s="3"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="15">
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="19">
         <v>1.0869</v>
       </c>
       <c r="T5" t="s">
@@ -1427,7 +1442,7 @@
       <c r="O7" s="7">
         <v>800000</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="15">
         <f t="shared" si="1"/>
         <v>1.25753515</v>
       </c>
@@ -1437,7 +1452,7 @@
       <c r="R7" s="7">
         <v>958941.73</v>
       </c>
-      <c r="S7" s="12">
+      <c r="S7" s="15">
         <v>1.0955</v>
       </c>
       <c r="T7" s="5"/>
@@ -1452,7 +1467,7 @@
       <c r="C9" s="3"/>
       <c r="E9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="N9" s="13">
+      <c r="N9" s="16">
         <v>1034393.13</v>
       </c>
       <c r="O9" s="3">
@@ -1491,7 +1506,7 @@
       <c r="H10" s="3">
         <v>430479.94</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="16">
         <v>1093859.91</v>
       </c>
       <c r="O10" s="3">
@@ -1537,7 +1552,7 @@
       <c r="L11" s="3">
         <v>272409.98</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="16">
         <v>1144503.28</v>
       </c>
       <c r="O11" s="3">
@@ -1580,7 +1595,7 @@
         <v>449593.74</v>
       </c>
       <c r="L12" s="3"/>
-      <c r="N12" s="13">
+      <c r="N12" s="16">
         <v>1144503.28</v>
       </c>
       <c r="O12" s="3">
@@ -1625,7 +1640,7 @@
       <c r="L13" s="3">
         <v>126667.79</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="16">
         <v>1162768.97</v>
       </c>
       <c r="O13" s="3">
@@ -1667,7 +1682,7 @@
       <c r="H14" s="3">
         <v>452487.27</v>
       </c>
-      <c r="N14" s="13">
+      <c r="N14" s="16">
         <v>1162768.97</v>
       </c>
       <c r="O14" s="3">
@@ -1687,46 +1702,52 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15">
+      <c r="A15" s="8">
         <v>20161230</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="9">
         <v>2854917.61</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="10">
         <v>356418.02</v>
       </c>
-      <c r="E15" s="3">
+      <c r="D15" s="8"/>
+      <c r="E15" s="10">
         <v>1329706.14</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="10">
         <v>712025.26</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3">
+      <c r="G15" s="10"/>
+      <c r="H15" s="10">
         <v>456768.19</v>
       </c>
-      <c r="N15" s="13">
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="7">
         <v>1212629.43</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="10">
         <v>800000</v>
       </c>
-      <c r="P15" s="1">
+      <c r="P15" s="17">
         <v>1.5158</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q15" s="10">
         <v>1642288.17</v>
       </c>
-      <c r="R15" s="3">
+      <c r="R15" s="10">
         <v>1358019.5</v>
       </c>
-      <c r="S15" s="1">
+      <c r="S15" s="17">
         <v>1.2093</v>
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="8">
+      <c r="A16" s="11">
         <v>42372</v>
       </c>
       <c r="B16" s="4">
@@ -1751,7 +1772,7 @@
       <c r="L16" s="3">
         <v>124038.7</v>
       </c>
-      <c r="N16" s="13">
+      <c r="N16" s="16">
         <v>1212629.43</v>
       </c>
       <c r="O16" s="3">
@@ -1794,7 +1815,7 @@
         <v>606768.19</v>
       </c>
       <c r="J17" s="3"/>
-      <c r="N17" s="13">
+      <c r="N17" s="16">
         <v>1212629.43</v>
       </c>
       <c r="O17" s="3">
@@ -1842,7 +1863,7 @@
       <c r="L18" s="3">
         <v>246305.42</v>
       </c>
-      <c r="N18" s="13">
+      <c r="N18" s="16">
         <v>1230552.72</v>
       </c>
       <c r="O18" s="3">
@@ -1894,7 +1915,7 @@
         <f>SUM(L3:L18)</f>
         <v>1728363.62</v>
       </c>
-      <c r="N19" s="13">
+      <c r="N19" s="16">
         <v>1230552.72</v>
       </c>
       <c r="O19" s="3">
@@ -1936,7 +1957,7 @@
         <v>622075.71</v>
       </c>
       <c r="J20" s="3"/>
-      <c r="N20" s="13">
+      <c r="N20" s="16">
         <v>1292267</v>
       </c>
       <c r="O20" s="3">
@@ -1977,9 +1998,8 @@
       <c r="H21" s="3">
         <v>656204.31</v>
       </c>
-      <c r="I21"/>
       <c r="J21" s="3"/>
-      <c r="N21" s="13">
+      <c r="N21" s="16">
         <v>1392989.46</v>
       </c>
       <c r="O21" s="3">
@@ -1998,21 +2018,95 @@
         <v>1.2915</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="4"/>
-      <c r="C22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+    <row r="22" spans="1:19">
+      <c r="A22">
+        <v>20170126</v>
+      </c>
+      <c r="B22" s="4">
+        <v>3745015.14</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1074975.14</v>
+      </c>
+      <c r="E22" s="3">
+        <v>982270</v>
+      </c>
+      <c r="F22" s="3">
+        <v>709911</v>
+      </c>
+      <c r="G22" s="3">
+        <v>309884</v>
+      </c>
+      <c r="H22" s="3">
+        <v>667975</v>
+      </c>
       <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="4"/>
-      <c r="C23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="N22" s="16">
+        <v>1461199.26</v>
+      </c>
+      <c r="O22" s="3">
+        <v>800000</v>
+      </c>
+      <c r="P22" s="1">
+        <v>1.8265</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>2283815.87</v>
+      </c>
+      <c r="R22" s="3">
+        <v>1728363.62</v>
+      </c>
+      <c r="S22" s="1">
+        <v>1.3214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="9">
+        <v>3745015.14</v>
+      </c>
+      <c r="C23" s="10">
+        <v>1074975.14</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="10">
+        <v>982270</v>
+      </c>
+      <c r="F23" s="10">
+        <v>709911</v>
+      </c>
+      <c r="G23" s="10">
+        <v>309884</v>
+      </c>
+      <c r="H23" s="10">
+        <v>667975</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="7">
+        <v>1461199.26</v>
+      </c>
+      <c r="O23" s="10">
+        <v>800000</v>
+      </c>
+      <c r="P23" s="17">
+        <v>1.8265</v>
+      </c>
+      <c r="Q23" s="10">
+        <v>2283815.87</v>
+      </c>
+      <c r="R23" s="10">
+        <v>1728363.62</v>
+      </c>
+      <c r="S23" s="17">
+        <v>1.3214</v>
+      </c>
+      <c r="T23" s="8"/>
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="4"/>
@@ -2023,155 +2117,155 @@
       <c r="J24" s="3"/>
     </row>
     <row r="25" spans="2:10">
-      <c r="B25" s="9"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="3"/>
       <c r="E25" s="3"/>
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="2:10">
-      <c r="B26" s="9"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="3"/>
       <c r="E26" s="3"/>
       <c r="J26" s="3"/>
     </row>
     <row r="27" spans="2:10">
-      <c r="B27" s="9"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="3"/>
       <c r="E27" s="3"/>
       <c r="J27" s="3"/>
     </row>
     <row r="28" spans="2:10">
-      <c r="B28" s="9"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="3"/>
       <c r="E28" s="3"/>
       <c r="J28" s="3"/>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="9"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="3"/>
       <c r="E29" s="3"/>
       <c r="J29" s="3"/>
     </row>
     <row r="30" spans="2:10">
-      <c r="B30" s="9"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="3"/>
       <c r="E30" s="3"/>
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="2:10">
-      <c r="B31" s="9"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="3"/>
       <c r="E31" s="3"/>
       <c r="J31" s="3"/>
     </row>
     <row r="32" spans="2:10">
-      <c r="B32" s="9"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="3"/>
       <c r="E32" s="3"/>
       <c r="J32" s="3"/>
     </row>
     <row r="33" spans="2:10">
-      <c r="B33" s="9"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="3"/>
       <c r="E33" s="3"/>
       <c r="J33" s="3"/>
     </row>
     <row r="34" spans="2:10">
-      <c r="B34" s="9"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="3"/>
       <c r="E34" s="3"/>
       <c r="J34" s="3"/>
     </row>
     <row r="35" spans="2:10">
-      <c r="B35" s="9"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="3"/>
       <c r="E35" s="3"/>
       <c r="J35" s="3"/>
     </row>
     <row r="36" spans="2:10">
-      <c r="B36" s="9"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="3"/>
       <c r="E36" s="3"/>
       <c r="J36" s="3"/>
     </row>
     <row r="37" spans="2:10">
-      <c r="B37" s="9"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="3"/>
       <c r="E37" s="3"/>
       <c r="J37" s="3"/>
     </row>
     <row r="38" spans="2:10">
-      <c r="B38" s="9"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="3"/>
       <c r="E38" s="3"/>
       <c r="J38" s="3"/>
     </row>
     <row r="39" spans="2:10">
-      <c r="B39" s="9"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="3"/>
       <c r="E39" s="3"/>
       <c r="J39" s="3"/>
     </row>
     <row r="40" spans="2:10">
-      <c r="B40" s="9"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="3"/>
       <c r="E40" s="3"/>
       <c r="J40" s="3"/>
     </row>
     <row r="41" spans="2:10">
-      <c r="B41" s="9"/>
+      <c r="B41" s="12"/>
       <c r="J41" s="3"/>
     </row>
     <row r="42" spans="2:10">
-      <c r="B42" s="9"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="3"/>
       <c r="E42" s="3"/>
       <c r="J42" s="3"/>
     </row>
     <row r="43" spans="2:10">
-      <c r="B43" s="9"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="3"/>
       <c r="E43" s="3"/>
       <c r="J43" s="3"/>
     </row>
     <row r="44" spans="2:10">
-      <c r="B44" s="9"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="3"/>
       <c r="E44" s="3"/>
       <c r="J44" s="3"/>
     </row>
     <row r="45" spans="2:10">
-      <c r="B45" s="9"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="3"/>
       <c r="E45" s="3"/>
       <c r="J45" s="3"/>
     </row>
     <row r="46" spans="2:10">
-      <c r="B46" s="9"/>
+      <c r="B46" s="12"/>
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="2:10">
-      <c r="B47" s="9"/>
+      <c r="B47" s="12"/>
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="2:10">
-      <c r="B48" s="9"/>
+      <c r="B48" s="12"/>
       <c r="J48" s="3"/>
     </row>
     <row r="49" spans="2:10">
-      <c r="B49" s="9"/>
+      <c r="B49" s="12"/>
       <c r="C49" s="3"/>
       <c r="E49" s="3"/>
       <c r="J49" s="3"/>
     </row>
     <row r="51" spans="11:18">
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-      <c r="Q51" s="14"/>
-      <c r="R51" s="14"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+      <c r="Q51" s="18"/>
+      <c r="R51" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update netvalue for Explorer
</commit_message>
<xml_diff>
--- a/ExplorerFund/NetValue/fund record.xlsx
+++ b/ExplorerFund/NetValue/fund record.xlsx
@@ -117,15 +117,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0000_);[Red]\(0.0000\)"/>
     <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
     <numFmt numFmtId="178" formatCode="#,##0.0_ "/>
-    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="180" formatCode="0.0000_ "/>
+    <numFmt numFmtId="179" formatCode="0.0000_ "/>
+    <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -159,10 +159,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -175,7 +175,85 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -196,78 +274,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -282,14 +289,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,55 +304,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,25 +466,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,97 +484,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,11 +498,76 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,73 +590,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -603,145 +603,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -785,10 +785,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -1112,8 +1112,8 @@
   <sheetPr/>
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27:T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2318,16 +2318,55 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:14">
-      <c r="B27" s="9"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+    <row r="27" spans="1:20">
+      <c r="A27">
+        <v>20170220</v>
+      </c>
+      <c r="B27" s="3">
+        <v>4226257</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1882701</v>
+      </c>
+      <c r="D27" s="3">
+        <v>832914</v>
+      </c>
+      <c r="E27" s="3">
+        <v>515736</v>
+      </c>
+      <c r="F27" s="3">
+        <v>327247</v>
+      </c>
+      <c r="G27" s="3">
+        <v>667659</v>
+      </c>
       <c r="H27" s="3"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9">
-        <f>N26+O26+R26</f>
-        <v>4107768.16</v>
+      <c r="L27" s="4">
+        <v>2.88</v>
+      </c>
+      <c r="M27">
+        <v>1.755</v>
+      </c>
+      <c r="N27" s="3">
+        <v>351000</v>
+      </c>
+      <c r="O27" s="3">
+        <v>1430534.39</v>
+      </c>
+      <c r="P27">
+        <v>666684.18</v>
+      </c>
+      <c r="Q27">
+        <v>2.1457</v>
+      </c>
+      <c r="R27" s="11">
+        <v>2444722.61</v>
+      </c>
+      <c r="S27" s="11">
+        <v>1748728.62</v>
+      </c>
+      <c r="T27" s="1">
+        <v>1.398</v>
       </c>
     </row>
     <row r="28" spans="2:14">

</xml_diff>

<commit_message>
update fund net value
</commit_message>
<xml_diff>
--- a/ExplorerFund/NetValue/fund record.xlsx
+++ b/ExplorerFund/NetValue/fund record.xlsx
@@ -116,16 +116,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="11">
+    <numFmt numFmtId="176" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.0000_);[Red]\(0.0000\)"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0.0_ "/>
-    <numFmt numFmtId="179" formatCode="0.0000_ "/>
-    <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="179" formatCode="#,##0.0_ "/>
+    <numFmt numFmtId="180" formatCode="#,##0.0000_ "/>
+    <numFmt numFmtId="181" formatCode="0.0000_ "/>
+    <numFmt numFmtId="182" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -152,15 +154,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,30 +182,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -219,9 +196,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,11 +211,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -260,28 +243,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -294,6 +256,46 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -304,6 +306,150 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -334,60 +480,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -395,96 +487,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,21 +497,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -522,17 +509,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -548,17 +529,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -587,11 +557,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -603,10 +605,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -615,186 +617,192 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="57" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="57" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1112,8 +1120,8 @@
   <sheetPr/>
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27:T27"/>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1128,7 +1136,7 @@
     <col min="9" max="9" width="12.125" customWidth="1"/>
     <col min="10" max="10" width="12.75" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="11.375" customWidth="1"/>
+    <col min="12" max="12" width="13.375" customWidth="1"/>
     <col min="13" max="13" width="10.125" customWidth="1"/>
     <col min="14" max="14" width="13.75" customWidth="1"/>
     <col min="15" max="15" width="16" customWidth="1"/>
@@ -1344,7 +1352,7 @@
       <c r="S4" s="3">
         <v>822018.44</v>
       </c>
-      <c r="T4" s="13">
+      <c r="T4" s="15">
         <f>0.0868942855166899+1</f>
         <v>1.08689428551669</v>
       </c>
@@ -1370,9 +1378,9 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="P5" s="3"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="13">
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="15">
         <v>1.0869</v>
       </c>
       <c r="U5" t="s">
@@ -1477,7 +1485,7 @@
       <c r="S7" s="7">
         <v>958941.73</v>
       </c>
-      <c r="T7" s="15">
+      <c r="T7" s="17">
         <v>1.0955</v>
       </c>
       <c r="U7" s="5"/>
@@ -1809,7 +1817,7 @@
       <c r="S15" s="7">
         <v>1358019.5</v>
       </c>
-      <c r="T15" s="15">
+      <c r="T15" s="17">
         <v>1.2093</v>
       </c>
     </row>
@@ -2156,7 +2164,7 @@
       <c r="S22" s="7">
         <v>1728363.62</v>
       </c>
-      <c r="T22" s="15">
+      <c r="T22" s="17">
         <v>1.3214</v>
       </c>
     </row>
@@ -2226,7 +2234,7 @@
       <c r="P24" s="11">
         <v>600000</v>
       </c>
-      <c r="Q24" s="16">
+      <c r="Q24" s="18">
         <v>2.0555</v>
       </c>
       <c r="R24" s="11">
@@ -2235,7 +2243,7 @@
       <c r="S24" s="11">
         <v>1728363.62</v>
       </c>
-      <c r="T24" s="16">
+      <c r="T24" s="18">
         <v>1.3703</v>
       </c>
     </row>
@@ -2311,7 +2319,7 @@
       <c r="S26" s="11">
         <v>1748728.62</v>
       </c>
-      <c r="T26" s="16">
+      <c r="T26" s="18">
         <v>1.3703</v>
       </c>
       <c r="U26" t="s">
@@ -2320,7 +2328,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27">
-        <v>20170220</v>
+        <v>20170226</v>
       </c>
       <c r="B27" s="3">
         <v>4226257</v>
@@ -2369,14 +2377,56 @@
         <v>1.398</v>
       </c>
     </row>
-    <row r="28" spans="2:14">
-      <c r="B28" s="9"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+    <row r="28" spans="1:20">
+      <c r="A28">
+        <v>20170303</v>
+      </c>
+      <c r="B28" s="4">
+        <v>4190964</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1790428</v>
+      </c>
+      <c r="D28" s="3">
+        <v>854446</v>
+      </c>
+      <c r="E28">
+        <v>515398</v>
+      </c>
+      <c r="F28">
+        <v>325642</v>
+      </c>
+      <c r="G28">
+        <v>705050</v>
+      </c>
       <c r="H28" s="3"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
+      <c r="L28" s="12">
+        <v>-0.835</v>
+      </c>
+      <c r="M28" s="13">
+        <v>1.74</v>
+      </c>
+      <c r="N28" s="3">
+        <v>348000</v>
+      </c>
+      <c r="O28" s="3">
+        <v>1418559.53</v>
+      </c>
+      <c r="P28">
+        <v>666684.18</v>
+      </c>
+      <c r="Q28">
+        <v>2.1278</v>
+      </c>
+      <c r="R28" s="11">
+        <v>2424262.49</v>
+      </c>
+      <c r="S28" s="11">
+        <v>1748728.62</v>
+      </c>
+      <c r="T28" s="1">
+        <v>1.3863</v>
+      </c>
     </row>
     <row r="29" spans="2:14">
       <c r="B29" s="9"/>
@@ -2565,14 +2615,14 @@
       <c r="N50" s="9"/>
     </row>
     <row r="51" spans="9:19">
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="12"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
-      <c r="R51" s="12"/>
-      <c r="S51" s="12"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update account for Explorer
</commit_message>
<xml_diff>
--- a/ExplorerFund/NetValue/fund record.xlsx
+++ b/ExplorerFund/NetValue/fund record.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
   <si>
     <t>日期</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 股东权益</t>
+  </si>
+  <si>
+    <t>1.483,961.03</t>
   </si>
 </sst>
 </file>
@@ -117,16 +120,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="11">
-    <numFmt numFmtId="176" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="177" formatCode="0.0000_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.0000_);[Red]\(0.0000\)"/>
     <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="179" formatCode="#,##0.0_ "/>
-    <numFmt numFmtId="180" formatCode="#,##0.0000_ "/>
-    <numFmt numFmtId="181" formatCode="0.0000_ "/>
+    <numFmt numFmtId="179" formatCode="0.00_ "/>
+    <numFmt numFmtId="180" formatCode="#,##0.0_ "/>
+    <numFmt numFmtId="181" formatCode="#,##0.0000_ "/>
     <numFmt numFmtId="182" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="22">
@@ -154,14 +157,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -182,6 +186,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -196,8 +224,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,18 +240,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -243,7 +265,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,46 +299,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -306,6 +309,138 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -324,24 +459,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -354,48 +471,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -415,78 +490,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,6 +500,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -509,11 +527,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -529,6 +553,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,43 +592,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,10 +608,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -617,192 +620,204 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="57" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="57" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1120,8 +1135,8 @@
   <sheetPr/>
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="K4" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1173,7 +1188,7 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
@@ -1352,7 +1367,7 @@
       <c r="S4" s="3">
         <v>822018.44</v>
       </c>
-      <c r="T4" s="15">
+      <c r="T4" s="13">
         <f>0.0868942855166899+1</f>
         <v>1.08689428551669</v>
       </c>
@@ -1378,9 +1393,9 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="P5" s="3"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="15">
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="13">
         <v>1.0869</v>
       </c>
       <c r="U5" t="s">
@@ -1461,7 +1476,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="6">
+      <c r="L7" s="12">
         <v>13.97</v>
       </c>
       <c r="M7">
@@ -1485,10 +1500,13 @@
       <c r="S7" s="7">
         <v>958941.73</v>
       </c>
-      <c r="T7" s="17">
+      <c r="T7" s="21">
         <v>1.0955</v>
       </c>
       <c r="U7" s="5"/>
+    </row>
+    <row r="8" spans="12:12">
+      <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9">
@@ -1500,7 +1518,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="L9" s="4">
+      <c r="L9" s="13">
         <v>2.148</v>
       </c>
       <c r="M9">
@@ -1548,7 +1566,7 @@
       <c r="G10" s="3">
         <v>430479.94</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="13">
         <v>4.39</v>
       </c>
       <c r="M10">
@@ -1603,7 +1621,7 @@
       <c r="J11" s="3">
         <v>272409.98</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="13">
         <v>3.56</v>
       </c>
       <c r="M11">
@@ -1655,7 +1673,7 @@
         <v>449593.74</v>
       </c>
       <c r="J12" s="3"/>
-      <c r="L12" s="4"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="3"/>
@@ -1701,7 +1719,7 @@
       <c r="J13" s="3">
         <v>126667.79</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="13">
         <v>1.15</v>
       </c>
       <c r="M13">
@@ -1752,6 +1770,7 @@
       <c r="G14" s="3">
         <v>452487.27</v>
       </c>
+      <c r="L14" s="13"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3">
         <v>600000</v>
@@ -1793,7 +1812,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15">
+      <c r="L15" s="13">
         <v>3.031</v>
       </c>
       <c r="M15">
@@ -1817,7 +1836,7 @@
       <c r="S15" s="7">
         <v>1358019.5</v>
       </c>
-      <c r="T15" s="17">
+      <c r="T15" s="21">
         <v>1.2093</v>
       </c>
     </row>
@@ -1847,6 +1866,7 @@
       <c r="J16" s="3">
         <v>124038.7</v>
       </c>
+      <c r="L16" s="13"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3">
         <v>600000</v>
@@ -1888,6 +1908,7 @@
         <v>606768.19</v>
       </c>
       <c r="H17" s="3"/>
+      <c r="L17" s="13"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3">
         <v>600000</v>
@@ -1931,7 +1952,7 @@
       <c r="J18" s="3">
         <v>246305.42</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="13">
         <v>1.01</v>
       </c>
       <c r="M18">
@@ -1992,6 +2013,7 @@
         <f>SUM(J3:J18)</f>
         <v>1728363.62</v>
       </c>
+      <c r="L19" s="13"/>
       <c r="M19">
         <v>1.4439</v>
       </c>
@@ -2038,7 +2060,7 @@
         <v>622075.71</v>
       </c>
       <c r="H20" s="3"/>
-      <c r="L20" s="4">
+      <c r="L20" s="13">
         <v>3.31</v>
       </c>
       <c r="M20">
@@ -2089,7 +2111,7 @@
         <v>656204.31</v>
       </c>
       <c r="H21" s="3"/>
-      <c r="L21" s="4">
+      <c r="L21" s="13">
         <v>5.19</v>
       </c>
       <c r="M21">
@@ -2140,7 +2162,7 @@
         <v>667975</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="L22" s="4">
+      <c r="L22" s="13">
         <v>3.3</v>
       </c>
       <c r="M22">
@@ -2149,7 +2171,7 @@
       <c r="N22" s="3">
         <v>324200</v>
       </c>
-      <c r="O22" s="11">
+      <c r="O22" s="14">
         <v>1136999.27</v>
       </c>
       <c r="P22" s="3">
@@ -2164,7 +2186,7 @@
       <c r="S22" s="7">
         <v>1728363.62</v>
       </c>
-      <c r="T22" s="17">
+      <c r="T22" s="21">
         <v>1.3214</v>
       </c>
     </row>
@@ -2194,6 +2216,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
+      <c r="L23" s="13"/>
       <c r="U23" s="5"/>
     </row>
     <row r="24" spans="1:20">
@@ -2219,7 +2242,7 @@
         <v>694072</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="L24" s="4">
+      <c r="L24" s="13">
         <v>5.28</v>
       </c>
       <c r="M24">
@@ -2231,19 +2254,19 @@
       <c r="O24" s="3">
         <v>1233323.18</v>
       </c>
-      <c r="P24" s="11">
+      <c r="P24" s="14">
         <v>600000</v>
       </c>
-      <c r="Q24" s="18">
+      <c r="Q24" s="22">
         <v>2.0555</v>
       </c>
-      <c r="R24" s="11">
+      <c r="R24" s="14">
         <v>2368302.82</v>
       </c>
-      <c r="S24" s="11">
+      <c r="S24" s="14">
         <v>1728363.62</v>
       </c>
-      <c r="T24" s="18">
+      <c r="T24" s="22">
         <v>1.3703</v>
       </c>
     </row>
@@ -2261,7 +2284,7 @@
       <c r="K25" t="s">
         <v>31</v>
       </c>
-      <c r="L25" s="4"/>
+      <c r="L25" s="13"/>
       <c r="M25" s="4"/>
       <c r="U25" t="s">
         <v>23</v>
@@ -2299,7 +2322,7 @@
       <c r="K26" t="s">
         <v>17</v>
       </c>
-      <c r="L26" s="4"/>
+      <c r="L26" s="13"/>
       <c r="M26" s="4"/>
       <c r="N26" s="3">
         <v>341200</v>
@@ -2313,13 +2336,13 @@
       <c r="Q26">
         <v>2.055</v>
       </c>
-      <c r="R26" s="11">
+      <c r="R26" s="14">
         <v>2396208.98</v>
       </c>
-      <c r="S26" s="11">
+      <c r="S26" s="14">
         <v>1748728.62</v>
       </c>
-      <c r="T26" s="18">
+      <c r="T26" s="22">
         <v>1.3703</v>
       </c>
       <c r="U26" t="s">
@@ -2349,7 +2372,7 @@
         <v>667659</v>
       </c>
       <c r="H27" s="3"/>
-      <c r="L27" s="4">
+      <c r="L27" s="13">
         <v>2.88</v>
       </c>
       <c r="M27">
@@ -2367,10 +2390,10 @@
       <c r="Q27">
         <v>2.1457</v>
       </c>
-      <c r="R27" s="11">
+      <c r="R27" s="14">
         <v>2444722.61</v>
       </c>
-      <c r="S27" s="11">
+      <c r="S27" s="14">
         <v>1748728.62</v>
       </c>
       <c r="T27" s="1">
@@ -2390,20 +2413,20 @@
       <c r="D28" s="3">
         <v>854446</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="9">
         <v>515398</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="9">
         <v>325642</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="9">
         <v>705050</v>
       </c>
       <c r="H28" s="3"/>
-      <c r="L28" s="12">
+      <c r="L28" s="13">
         <v>-0.835</v>
       </c>
-      <c r="M28" s="13">
+      <c r="M28" s="15">
         <v>1.74</v>
       </c>
       <c r="N28" s="3">
@@ -2418,211 +2441,282 @@
       <c r="Q28">
         <v>2.1278</v>
       </c>
-      <c r="R28" s="11">
+      <c r="R28" s="14">
         <v>2424262.49</v>
       </c>
-      <c r="S28" s="11">
+      <c r="S28" s="14">
         <v>1748728.62</v>
       </c>
       <c r="T28" s="1">
         <v>1.3863</v>
       </c>
     </row>
-    <row r="29" spans="2:14">
-      <c r="B29" s="9"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+    <row r="29" spans="1:20">
+      <c r="A29">
+        <v>201703017</v>
+      </c>
+      <c r="B29" s="3">
+        <f>C29+D29+E29+F29+D31+G29</f>
+        <v>4231191</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1128589</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1166835</v>
+      </c>
+      <c r="E29" s="9">
+        <v>829521</v>
+      </c>
+      <c r="F29" s="9">
+        <v>331121</v>
+      </c>
+      <c r="G29" s="9">
+        <v>775125</v>
+      </c>
       <c r="H29" s="3"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-    </row>
-    <row r="30" spans="2:14">
-      <c r="B30" s="9"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
+      <c r="L29" s="13">
+        <v>0.1167</v>
+      </c>
+      <c r="M29" s="16">
+        <v>1.757</v>
+      </c>
+      <c r="N29" s="10"/>
+      <c r="Q29">
+        <v>2.1482</v>
+      </c>
+      <c r="T29" s="1">
+        <v>1.3996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30">
+        <v>20170324</v>
+      </c>
+      <c r="B30" s="3">
+        <f>SUM(C30:G30)</f>
+        <v>4330508</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1125254</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1199443</v>
+      </c>
+      <c r="E30" s="9">
+        <v>840362</v>
+      </c>
+      <c r="F30" s="9">
+        <v>333994</v>
+      </c>
+      <c r="G30" s="9">
+        <v>831455</v>
+      </c>
+      <c r="L30" s="13">
+        <v>2.4667</v>
+      </c>
+      <c r="M30" s="17">
+        <v>1.7983</v>
+      </c>
+      <c r="N30" s="10">
+        <v>359660</v>
+      </c>
+      <c r="O30" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="P30">
+        <v>666684.18</v>
+      </c>
+      <c r="Q30">
+        <v>2.2259</v>
+      </c>
+      <c r="R30" s="3">
+        <v>2486866.97</v>
+      </c>
+      <c r="S30" s="14">
+        <v>1748728.62</v>
+      </c>
+      <c r="T30" s="1">
+        <v>1.4221</v>
+      </c>
     </row>
     <row r="31" spans="2:14">
-      <c r="B31" s="9"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
     </row>
     <row r="32" spans="2:14">
-      <c r="B32" s="9"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
     </row>
     <row r="33" spans="2:14">
-      <c r="B33" s="9"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
     </row>
     <row r="34" spans="2:14">
-      <c r="B34" s="9"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
     </row>
     <row r="35" spans="2:14">
-      <c r="B35" s="9"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="9"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
     </row>
     <row r="37" spans="2:14">
-      <c r="B37" s="9"/>
+      <c r="B37" s="10"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
     </row>
     <row r="38" spans="2:14">
-      <c r="B38" s="9"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
     </row>
     <row r="39" spans="2:14">
-      <c r="B39" s="9"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
     </row>
     <row r="40" spans="2:14">
-      <c r="B40" s="9"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
     </row>
     <row r="41" spans="2:14">
-      <c r="B41" s="9"/>
+      <c r="B41" s="10"/>
       <c r="H41" s="3"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
     </row>
     <row r="42" spans="2:14">
-      <c r="B42" s="9"/>
+      <c r="B42" s="10"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
     </row>
     <row r="43" spans="2:14">
-      <c r="B43" s="9"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
     </row>
     <row r="44" spans="2:14">
-      <c r="B44" s="9"/>
+      <c r="B44" s="10"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
     </row>
     <row r="45" spans="2:14">
-      <c r="B45" s="9"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
     </row>
     <row r="46" spans="2:14">
-      <c r="B46" s="9"/>
+      <c r="B46" s="10"/>
       <c r="H46" s="3"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
     </row>
     <row r="47" spans="2:14">
-      <c r="B47" s="9"/>
+      <c r="B47" s="10"/>
       <c r="H47" s="3"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
     </row>
     <row r="48" spans="2:14">
-      <c r="B48" s="9"/>
+      <c r="B48" s="10"/>
       <c r="H48" s="3"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
     </row>
     <row r="49" spans="2:14">
-      <c r="B49" s="9"/>
+      <c r="B49" s="10"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="9"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
     </row>
     <row r="50" spans="12:14">
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="9"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
     </row>
     <row r="51" spans="9:19">
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="9"/>
-      <c r="M51" s="9"/>
-      <c r="N51" s="9"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="14"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="R51" s="19"/>
+      <c r="S51" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update net value for Explorer
</commit_message>
<xml_diff>
--- a/ExplorerFund/NetValue/fund record.xlsx
+++ b/ExplorerFund/NetValue/fund record.xlsx
@@ -120,15 +120,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="11">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.0000_);[Red]\(0.0000\)"/>
-    <numFmt numFmtId="177" formatCode="0.0000_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="179" formatCode="0.00_ "/>
-    <numFmt numFmtId="180" formatCode="#,##0.0_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="178" formatCode="0.00_ "/>
+    <numFmt numFmtId="179" formatCode="#,##0.0_ "/>
+    <numFmt numFmtId="180" formatCode="0.0000_ "/>
     <numFmt numFmtId="181" formatCode="#,##0.0000_ "/>
     <numFmt numFmtId="182" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
@@ -763,34 +763,34 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -805,8 +805,8 @@
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
@@ -1135,8 +1135,8 @@
   <sheetPr/>
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K4" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" topLeftCell="K10" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2456,7 +2456,7 @@
         <v>201703017</v>
       </c>
       <c r="B29" s="3">
-        <f>C29+D29+E29+F29+D31+G29</f>
+        <f t="shared" ref="B29:B31" si="1">SUM(C29:G29)</f>
         <v>4231191</v>
       </c>
       <c r="C29" s="3">
@@ -2474,7 +2474,6 @@
       <c r="G29" s="9">
         <v>775125</v>
       </c>
-      <c r="H29" s="3"/>
       <c r="L29" s="13">
         <v>0.1167</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>20170324</v>
       </c>
       <c r="B30" s="3">
-        <f>SUM(C30:G30)</f>
+        <f t="shared" si="1"/>
         <v>4330508</v>
       </c>
       <c r="C30" s="3">
@@ -2518,10 +2517,10 @@
       <c r="M30" s="17">
         <v>1.7983</v>
       </c>
-      <c r="N30" s="10">
+      <c r="N30" s="4">
         <v>359660</v>
       </c>
-      <c r="O30" s="18" t="s">
+      <c r="O30" s="16" t="s">
         <v>32</v>
       </c>
       <c r="P30">
@@ -2540,30 +2539,114 @@
         <v>1.4221</v>
       </c>
     </row>
-    <row r="31" spans="2:14">
-      <c r="B31" s="10"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-    </row>
-    <row r="32" spans="2:14">
-      <c r="B32" s="10"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
+    <row r="31" spans="1:20">
+      <c r="A31">
+        <v>20170331</v>
+      </c>
+      <c r="B31" s="3">
+        <f t="shared" si="1"/>
+        <v>4445190</v>
+      </c>
+      <c r="C31" s="3">
+        <v>549872</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1531988</v>
+      </c>
+      <c r="E31" s="9">
+        <v>1134817</v>
+      </c>
+      <c r="F31" s="9">
+        <v>341227</v>
+      </c>
+      <c r="G31" s="9">
+        <v>887286</v>
+      </c>
+      <c r="L31" s="18">
+        <v>2.6482</v>
+      </c>
+      <c r="M31" s="18">
+        <v>1.8459</v>
+      </c>
+      <c r="N31" s="4">
+        <v>369180</v>
+      </c>
+      <c r="O31" s="3">
+        <v>1542454.59</v>
+      </c>
+      <c r="P31">
+        <v>666684.18</v>
+      </c>
+      <c r="Q31">
+        <v>2.3136</v>
+      </c>
+      <c r="R31" s="3">
+        <v>2533555.41</v>
+      </c>
+      <c r="S31" s="14">
+        <v>1748728.62</v>
+      </c>
+      <c r="T31" s="1">
+        <v>1.4488</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32">
+        <v>20170407</v>
+      </c>
+      <c r="B32" s="3">
+        <f>SUM(C32:G32)</f>
+        <v>4607171</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1082128</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1621269</v>
+      </c>
+      <c r="E32" s="3">
+        <v>633138</v>
+      </c>
+      <c r="F32" s="9">
+        <v>349038</v>
+      </c>
+      <c r="G32" s="9">
+        <v>921598</v>
+      </c>
+      <c r="L32" s="18">
+        <v>3.644</v>
+      </c>
+      <c r="M32" s="18">
+        <v>1.9132</v>
+      </c>
+      <c r="N32" s="4">
+        <v>382640</v>
+      </c>
+      <c r="O32" s="3">
+        <v>1626348</v>
+      </c>
+      <c r="P32">
+        <v>666684.18</v>
+      </c>
+      <c r="Q32">
+        <v>2.4395</v>
+      </c>
+      <c r="R32" s="3">
+        <v>2598183.33</v>
+      </c>
+      <c r="S32" s="14">
+        <v>1748728.62</v>
+      </c>
+      <c r="T32" s="1">
+        <v>1.4858</v>
+      </c>
     </row>
     <row r="33" spans="2:14">
       <c r="B33" s="10"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="L33" s="10"/>
+      <c r="L33" s="18"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
     </row>
@@ -2572,7 +2655,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="L34" s="10"/>
+      <c r="L34" s="18"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
     </row>
@@ -2581,7 +2664,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="L35" s="10"/>
+      <c r="L35" s="18"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
     </row>
@@ -2590,7 +2673,7 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="L36" s="10"/>
+      <c r="L36" s="18"/>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
     </row>

</xml_diff>

<commit_message>
update net value for Explore
</commit_message>
<xml_diff>
--- a/ExplorerFund/NetValue/fund record.xlsx
+++ b/ExplorerFund/NetValue/fund record.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20370" windowHeight="9000"/>
+    <workbookView windowWidth="20400" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <t>上期顾85</t>
   </si>
   <si>
-    <t>上期09</t>
+    <t>上期109</t>
   </si>
   <si>
     <t>郑商日盘权益</t>
@@ -123,17 +123,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="11">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0.0000_);[Red]\(0.0000\)"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.0000_);[Red]\(0.0000\)"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
-    <numFmt numFmtId="179" formatCode="#,##0.0_ "/>
-    <numFmt numFmtId="180" formatCode="0.0000_ "/>
-    <numFmt numFmtId="181" formatCode="#,##0.0000_ "/>
-    <numFmt numFmtId="182" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="179" formatCode="#,##0.0000_ "/>
+    <numFmt numFmtId="180" formatCode="0.00_ "/>
+    <numFmt numFmtId="181" formatCode="#,##0.0_ "/>
+    <numFmt numFmtId="182" formatCode="0.0000_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -161,29 +161,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,6 +197,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -227,19 +227,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -267,32 +280,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -312,7 +312,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -330,19 +354,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,13 +408,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,97 +426,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -480,7 +462,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -492,7 +480,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,6 +531,50 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -559,50 +603,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -614,7 +614,7 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -623,133 +623,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -757,7 +757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="57" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -766,13 +766,13 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -781,46 +781,46 @@
     <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -876,6 +876,11 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1129,17 +1134,16 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:V51"/>
+  <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="S35" sqref="S35"/>
+    <sheetView tabSelected="1" topLeftCell="M22" workbookViewId="0">
+      <selection activeCell="U49" sqref="U49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2481,7 +2485,7 @@
         <v>201703017</v>
       </c>
       <c r="B29" s="3">
-        <f t="shared" ref="B29:B34" si="1">SUM(C29:H29)</f>
+        <f t="shared" ref="B29:B42" si="1">SUM(C29:H29)</f>
         <v>4231191</v>
       </c>
       <c r="C29" s="3">
@@ -2780,7 +2784,7 @@
         <v>20170428</v>
       </c>
       <c r="B35" s="3">
-        <f>SUM(C35:H35)</f>
+        <f t="shared" si="1"/>
         <v>5106178</v>
       </c>
       <c r="C35" s="3">
@@ -2829,66 +2833,342 @@
         <v>1.5975</v>
       </c>
     </row>
-    <row r="36" spans="2:15">
-      <c r="B36" s="10"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="10"/>
+    <row r="36" spans="1:21">
+      <c r="A36">
+        <v>20170505</v>
+      </c>
+      <c r="B36" s="3">
+        <f t="shared" si="1"/>
+        <v>5012006</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1071144</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1159614</v>
+      </c>
+      <c r="E36" s="9">
+        <v>1238581</v>
+      </c>
+      <c r="F36" s="9">
+        <v>399541</v>
+      </c>
+      <c r="G36" s="9">
+        <v>199975</v>
+      </c>
+      <c r="H36" s="9">
+        <v>943151</v>
+      </c>
+      <c r="M36" s="18">
+        <v>-1.8443</v>
+      </c>
+      <c r="N36" s="18">
+        <v>2.0812</v>
+      </c>
       <c r="O36" s="10"/>
-    </row>
-    <row r="37" spans="2:15">
-      <c r="B37" s="10"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
+      <c r="R36">
+        <v>2.7804</v>
+      </c>
+      <c r="U36" s="1">
+        <v>1.568</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37">
+        <v>20170505</v>
+      </c>
+      <c r="B37" s="3">
+        <f t="shared" si="1"/>
+        <v>5094463</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1090948</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1182876</v>
+      </c>
+      <c r="E37" s="9">
+        <v>1251553</v>
+      </c>
+      <c r="F37" s="9">
+        <v>396282</v>
+      </c>
+      <c r="G37" s="9">
+        <v>199975</v>
+      </c>
+      <c r="H37" s="9">
+        <v>972829</v>
+      </c>
+      <c r="M37" s="18">
+        <v>1.6452</v>
+      </c>
+      <c r="N37" s="18">
+        <v>2.1154</v>
+      </c>
       <c r="O37" s="10"/>
-    </row>
-    <row r="38" spans="2:15">
-      <c r="B38" s="10"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-    </row>
-    <row r="39" spans="2:15">
-      <c r="B39" s="10"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-    </row>
-    <row r="40" spans="2:15">
-      <c r="B40" s="10"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-    </row>
-    <row r="41" spans="2:15">
-      <c r="B41" s="10"/>
-      <c r="I41" s="3"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-    </row>
-    <row r="42" spans="2:15">
-      <c r="B42" s="10"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
+      <c r="R37">
+        <v>2.8261</v>
+      </c>
+      <c r="U37" s="1">
+        <v>1.5937</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38">
+        <v>20170526</v>
+      </c>
+      <c r="B38" s="3">
+        <f t="shared" si="1"/>
+        <v>5144745</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1083186</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1150995</v>
+      </c>
+      <c r="E38" s="9">
+        <v>1213800</v>
+      </c>
+      <c r="F38" s="9">
+        <v>392781</v>
+      </c>
+      <c r="G38" s="9">
+        <v>199975</v>
+      </c>
+      <c r="H38" s="9">
+        <v>1104008</v>
+      </c>
+      <c r="M38" s="18">
+        <v>0.987</v>
+      </c>
+      <c r="N38" s="18">
+        <v>2.1363</v>
+      </c>
+      <c r="O38" s="4">
+        <v>427260</v>
+      </c>
+      <c r="P38" s="3">
+        <v>1904590</v>
+      </c>
+      <c r="Q38">
+        <v>666684.18</v>
+      </c>
+      <c r="R38">
+        <v>2.8568</v>
+      </c>
+      <c r="S38" s="3">
+        <v>2812895</v>
+      </c>
+      <c r="T38" s="14">
+        <v>1748728.62</v>
+      </c>
+      <c r="U38" s="1">
+        <v>1.6085</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39">
+        <v>20170609</v>
+      </c>
+      <c r="B39" s="3">
+        <f t="shared" si="1"/>
+        <v>5328915</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1088532</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1157785</v>
+      </c>
+      <c r="E39" s="9">
+        <v>1283456</v>
+      </c>
+      <c r="F39" s="9">
+        <v>393042</v>
+      </c>
+      <c r="G39" s="9">
+        <v>210678</v>
+      </c>
+      <c r="H39" s="9">
+        <v>1195422</v>
+      </c>
+      <c r="M39" s="18">
+        <v>3.5798</v>
+      </c>
+      <c r="N39" s="18">
+        <v>2.2127</v>
+      </c>
+      <c r="O39" s="4">
+        <v>442540</v>
+      </c>
+      <c r="P39" s="3">
+        <v>2003071</v>
+      </c>
+      <c r="Q39">
+        <v>666684.18</v>
+      </c>
+      <c r="R39">
+        <v>3.0045</v>
+      </c>
+      <c r="S39" s="3">
+        <v>2883304</v>
+      </c>
+      <c r="T39" s="14">
+        <v>1748728.62</v>
+      </c>
+      <c r="U39" s="1">
+        <v>1.6488</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24">
+      <c r="A40">
+        <v>20170616</v>
+      </c>
+      <c r="B40" s="3">
+        <f t="shared" si="1"/>
+        <v>5336864</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1060387</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1172583</v>
+      </c>
+      <c r="E40" s="9">
+        <v>1305794</v>
+      </c>
+      <c r="F40" s="9">
+        <v>402725</v>
+      </c>
+      <c r="G40" s="9">
+        <v>209681</v>
+      </c>
+      <c r="H40" s="9">
+        <v>1185694</v>
+      </c>
+      <c r="M40" s="18">
+        <v>0.1492</v>
+      </c>
+      <c r="N40" s="18">
+        <v>2.216</v>
+      </c>
+      <c r="O40" s="4">
+        <v>443200</v>
+      </c>
+      <c r="P40" s="3">
+        <v>2007349</v>
+      </c>
+      <c r="Q40">
+        <v>666684.18</v>
+      </c>
+      <c r="R40">
+        <v>3.0109</v>
+      </c>
+      <c r="S40" s="3">
+        <v>2886315</v>
+      </c>
+      <c r="T40" s="14">
+        <v>1748728.62</v>
+      </c>
+      <c r="U40">
+        <v>1.6505</v>
+      </c>
+      <c r="W40" s="3"/>
+      <c r="X40" s="14"/>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41">
+        <v>20170623</v>
+      </c>
+      <c r="B41" s="3">
+        <f t="shared" si="1"/>
+        <v>5339509</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1062522</v>
+      </c>
+      <c r="D41" s="3">
+        <v>168237</v>
+      </c>
+      <c r="E41" s="9">
+        <v>1299004</v>
+      </c>
+      <c r="F41" s="9">
+        <v>394191</v>
+      </c>
+      <c r="G41" s="9">
+        <v>1214931</v>
+      </c>
+      <c r="H41" s="9">
+        <v>1200624</v>
+      </c>
+      <c r="M41" s="18">
+        <v>0.049</v>
+      </c>
+      <c r="N41" s="18"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="3"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="14"/>
+      <c r="U41"/>
+    </row>
+    <row r="42" spans="1:21">
+      <c r="A42">
+        <v>20170630</v>
+      </c>
+      <c r="B42" s="3">
+        <f t="shared" si="1"/>
+        <v>5311702</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1056367</v>
+      </c>
+      <c r="D42" s="3">
+        <v>168237</v>
+      </c>
+      <c r="E42" s="9">
+        <v>1267231</v>
+      </c>
+      <c r="F42" s="9">
+        <v>393210</v>
+      </c>
+      <c r="G42" s="9">
+        <v>1204791</v>
+      </c>
+      <c r="H42" s="9">
+        <v>1221866</v>
+      </c>
+      <c r="I42"/>
+      <c r="M42" s="18">
+        <v>-0.4714</v>
+      </c>
+      <c r="N42" s="18">
+        <v>2.2055</v>
+      </c>
+      <c r="O42" s="4">
+        <v>443200</v>
+      </c>
+      <c r="P42" s="3">
+        <v>2007349</v>
+      </c>
+      <c r="Q42">
+        <v>666684.18</v>
+      </c>
+      <c r="R42">
+        <v>2.9967</v>
+      </c>
+      <c r="S42" s="3">
+        <v>2886315</v>
+      </c>
+      <c r="T42" s="14">
+        <v>1748728.62</v>
+      </c>
+      <c r="U42">
+        <v>1.6427</v>
+      </c>
     </row>
     <row r="43" spans="2:15">
       <c r="B43" s="10"/>

</xml_diff>